<commit_message>
fix python script, generate xlsx file and update README
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-3.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-3.xlsx
@@ -368,7 +368,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>to go &lt;small&gt;(&lt;em&gt;destination&lt;/em&gt; に/へ)&lt;/small&gt;</t>
+          <t>to go (destination に/へ)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -380,7 +380,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>to go back; to return &lt;small&gt;(&lt;em&gt;destination&lt;/em&gt; に/へ)&lt;/small&gt;</t>
+          <t>to go back; to return (destination に/へ)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -392,7 +392,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>to listen; to hear &lt;small&gt;(～を)&lt;/small&gt;</t>
+          <t>to listen; to hear (～を)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -404,7 +404,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>to drink &lt;small&gt;(～を)&lt;/small&gt;</t>
+          <t>to drink (～を)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -416,7 +416,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>to speak; to talk &lt;small&gt;(&lt;em&gt;language&lt;/em&gt; を/で)&lt;/small&gt;</t>
+          <t>to speak; to talk (language を/で)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -428,7 +428,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>to read &lt;small&gt;(～を)&lt;/small&gt;</t>
+          <t>to read (～を)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -968,7 +968,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>to eat &lt;small&gt;(～を)&lt;/small&gt;</t>
+          <t>to eat (～を)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>to see; to look at; to watch &lt;small&gt;(～を)&lt;/small&gt;</t>
+          <t>to see; to look at; to watch (～を)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1004,7 +1004,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>to come &lt;small&gt;(&lt;em&gt;destination&lt;/em&gt; に/へ)&lt;/small&gt;</t>
+          <t>to come (destination に/へ)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1016,7 +1016,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>to do &lt;small&gt;(～を)&lt;/small&gt;</t>
+          <t>to do (～を)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1028,7 +1028,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>to study &lt;small&gt;(～を)&lt;/small&gt;</t>
+          <t>to study (～を)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">

</xml_diff>